<commit_message>
working on manager annual sells
</commit_message>
<xml_diff>
--- a/application/plugins/Reports_manager_annual_sells/views/Reports_manager_annual_sells.xlsx
+++ b/application/plugins/Reports_manager_annual_sells/views/Reports_manager_annual_sells.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4704" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="5820" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Отчет" sheetId="1" r:id="rId1"/>
@@ -664,6 +664,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -673,27 +721,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -711,36 +741,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1049,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,13 +1061,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -1075,263 +1075,263 @@
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="38" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="38"/>
+      <c r="E2" s="23"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="38" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="38"/>
+      <c r="E3" s="23"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="38" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="38"/>
+      <c r="E4" s="23"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="38" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="23"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="38" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="38"/>
+      <c r="E6" s="23"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="41" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="E7" s="38"/>
+      <c r="E7" s="23"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="39" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="22"/>
+      <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="39" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E9" s="22"/>
+      <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="26" t="s">
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="22"/>
+      <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="26" t="s">
+      <c r="B11" s="40"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="22"/>
+      <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="26" t="s">
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="22"/>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="20" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="22"/>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="20" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="22"/>
+      <c r="E14" s="18"/>
     </row>
     <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:27" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
-      <c r="X17" s="35"/>
-      <c r="Y17" s="35"/>
-      <c r="Z17" s="35"/>
-      <c r="AA17" s="36"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="29"/>
+      <c r="AA17" s="30"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19" t="s">
+      <c r="C18" s="24"/>
+      <c r="D18" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19" t="s">
+      <c r="E18" s="24"/>
+      <c r="F18" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19" t="s">
+      <c r="G18" s="24"/>
+      <c r="H18" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19" t="s">
+      <c r="I18" s="24"/>
+      <c r="J18" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19" t="s">
+      <c r="K18" s="24"/>
+      <c r="L18" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19" t="s">
+      <c r="M18" s="24"/>
+      <c r="N18" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19" t="s">
+      <c r="O18" s="24"/>
+      <c r="P18" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19" t="s">
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19" t="s">
+      <c r="S18" s="24"/>
+      <c r="T18" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="U18" s="19"/>
-      <c r="V18" s="19" t="s">
+      <c r="U18" s="24"/>
+      <c r="V18" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="W18" s="19"/>
-      <c r="X18" s="19" t="s">
+      <c r="W18" s="24"/>
+      <c r="X18" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="Y18" s="19"/>
-      <c r="Z18" s="19" t="s">
+      <c r="Y18" s="24"/>
+      <c r="Z18" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AA18" s="32"/>
+      <c r="AA18" s="26"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1608,32 +1608,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="X18:Y18"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="A17:AA17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="T18:U18"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="A2:C2"/>
@@ -1650,6 +1624,32 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="A17:AA17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="47" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
awaiting & reserved columns in excel
</commit_message>
<xml_diff>
--- a/application/plugins/Reports_manager_annual_sells/views/Reports_manager_annual_sells.xlsx
+++ b/application/plugins/Reports_manager_annual_sells/views/Reports_manager_annual_sells.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="6936" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Отчет" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Отчет!$A$1:$AA$22</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -292,9 +292,6 @@
     <t>{$v-&gt;rows[]-&gt;sum}</t>
   </si>
   <si>
-    <t>Год</t>
-  </si>
-  <si>
     <t>Группировать по клиентам</t>
   </si>
   <si>
@@ -311,6 +308,9 @@
   </si>
   <si>
     <t>{$v-&gt;input-&gt;include_vat}</t>
+  </si>
+  <si>
+    <t>Итого</t>
   </si>
 </sst>
 </file>
@@ -664,83 +664,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1050,7 +1050,7 @@
   <dimension ref="A1:AA22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,13 +1061,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -1075,263 +1075,263 @@
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="23" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="23"/>
+      <c r="E2" s="32"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="23" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="23"/>
+      <c r="E3" s="32"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="23" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="32"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="23" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="32"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="23" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="32"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="32"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="22"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="22"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="36" t="s">
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="18"/>
+      <c r="E10" s="22"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="36" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="18"/>
+      <c r="E11" s="22"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="36" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="18"/>
+      <c r="E12" s="22"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="25" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="18"/>
+      <c r="E13" s="22"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="25" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="18"/>
+      <c r="E14" s="22"/>
     </row>
     <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:27" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="29"/>
-      <c r="T17" s="29"/>
-      <c r="U17" s="29"/>
-      <c r="V17" s="29"/>
-      <c r="W17" s="29"/>
-      <c r="X17" s="29"/>
-      <c r="Y17" s="29"/>
-      <c r="Z17" s="29"/>
-      <c r="AA17" s="30"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="36"/>
+      <c r="W17" s="36"/>
+      <c r="X17" s="36"/>
+      <c r="Y17" s="36"/>
+      <c r="Z17" s="36"/>
+      <c r="AA17" s="37"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24" t="s">
+      <c r="B18" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24" t="s">
+      <c r="E18" s="19"/>
+      <c r="F18" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24" t="s">
+      <c r="G18" s="19"/>
+      <c r="H18" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24" t="s">
+      <c r="I18" s="19"/>
+      <c r="J18" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24" t="s">
+      <c r="K18" s="19"/>
+      <c r="L18" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24" t="s">
+      <c r="M18" s="19"/>
+      <c r="N18" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24" t="s">
+      <c r="O18" s="19"/>
+      <c r="P18" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24" t="s">
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24" t="s">
+      <c r="S18" s="19"/>
+      <c r="T18" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24" t="s">
+      <c r="U18" s="19"/>
+      <c r="V18" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24" t="s">
+      <c r="W18" s="19"/>
+      <c r="X18" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24" t="s">
+      <c r="Y18" s="19"/>
+      <c r="Z18" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="AA18" s="26"/>
+      <c r="AA18" s="33"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A19" s="31"/>
+      <c r="A19" s="38"/>
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1608,6 +1608,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="A17:AA17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="T18:U18"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="A2:C2"/>
@@ -1624,32 +1650,6 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="X18:Y18"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="A17:AA17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="47" orientation="landscape" r:id="rId1"/>

</xml_diff>